<commit_message>
atualizações de funções de tratamento das colunas
</commit_message>
<xml_diff>
--- a/python/scripts/metadado.xlsx
+++ b/python/scripts/metadado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DE04/dataops/de04_dataops/aula02/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\dataops\aula03\de04_dataops\python\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_AD4D361C20488DEA4E38A0B7F41969B45ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8F9203-BC21-47CF-A020-10B26CA3D996}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED846C4-E13D-4FD2-9154-4934A3F8213B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2985" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>tabela</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>dob.date</t>
+  </si>
+  <si>
+    <t>rua</t>
+  </si>
+  <si>
+    <t>rua do endereço do indivíduo</t>
+  </si>
+  <si>
+    <t>limpa_texto</t>
+  </si>
+  <si>
+    <t>location.street.name</t>
   </si>
 </sst>
 </file>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:O10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +513,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -529,6 +543,9 @@
       <c r="G2">
         <v>0</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -552,6 +569,9 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -575,6 +595,9 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -598,6 +621,9 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -621,6 +647,9 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -644,6 +673,9 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -653,19 +685,22 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="G8">
         <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -676,19 +711,22 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -699,23 +737,52 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="2"/>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>